<commit_message>
Cambios en la base de datos
</commit_message>
<xml_diff>
--- a/Vistas.xlsx
+++ b/Vistas.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Desktop\Juan\UTN\Programacion 3\Repo_TPC\TPC-Equipo-8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5097CB-5DE0-4348-9DE8-70D57B1052F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92176DCA-2ACA-41D0-B5F1-5DEF62B737B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="741" activeTab="4" xr2:uid="{E07B4131-C04B-4E1D-A879-36A85FE57CE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="741" firstSheet="3" activeTab="6" xr2:uid="{E07B4131-C04B-4E1D-A879-36A85FE57CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
     <sheet name="Donante - Home" sheetId="2" r:id="rId2"/>
     <sheet name="Donante - DetalleFilial" sheetId="3" r:id="rId3"/>
     <sheet name="Donante - Publicaciones" sheetId="5" r:id="rId4"/>
-    <sheet name="Donante - Perfil" sheetId="4" r:id="rId5"/>
-    <sheet name="Filial - Home" sheetId="6" r:id="rId6"/>
-    <sheet name="Filial - GestionDonantes" sheetId="7" r:id="rId7"/>
-    <sheet name="Filial - GestionPublicaciones" sheetId="8" r:id="rId8"/>
-    <sheet name="Filial - PerfilFilial" sheetId="9" r:id="rId9"/>
-    <sheet name="Admin - GestionFiliales" sheetId="10" r:id="rId10"/>
-    <sheet name="Admin - GestionPublicaciones" sheetId="11" r:id="rId11"/>
-    <sheet name="Admin - Perfil" sheetId="12" r:id="rId12"/>
+    <sheet name="Declaracion Jurada" sheetId="13" r:id="rId5"/>
+    <sheet name="Donante - Perfil" sheetId="4" r:id="rId6"/>
+    <sheet name="Filial - Home" sheetId="6" r:id="rId7"/>
+    <sheet name="Filial - GestionDonantes" sheetId="7" r:id="rId8"/>
+    <sheet name="Filial - GestionPublicaciones" sheetId="8" r:id="rId9"/>
+    <sheet name="Filial - PerfilFilial" sheetId="9" r:id="rId10"/>
+    <sheet name="Admin - GestionFiliales" sheetId="10" r:id="rId11"/>
+    <sheet name="Admin - GestionPublicaciones" sheetId="11" r:id="rId12"/>
+    <sheet name="Admin - Perfil" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="112">
   <si>
     <t>FILIAL</t>
   </si>
@@ -329,6 +330,60 @@
   </si>
   <si>
     <t>FechaLimite</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>Crear Cuenta</t>
+  </si>
+  <si>
+    <t>Ya tengo Cuenta</t>
+  </si>
+  <si>
+    <t>txtBox</t>
+  </si>
+  <si>
+    <t>UNA VEZ QUE TOQUES EL BOTON DONAR</t>
+  </si>
+  <si>
+    <t>TE MANDA A UN FORMS</t>
+  </si>
+  <si>
+    <t>DECLARACION JURADA</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>Grupo Sanguineo</t>
+  </si>
+  <si>
+    <t>Fecha Nacimiento</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>Udonaste en los ultimos dos meses? SI/NO</t>
+  </si>
+  <si>
+    <t>6 meses desde ultimo tatuaje SI/NO</t>
+  </si>
+  <si>
+    <t>Dormir mas de 6 horas y presentate habiendo desayunado/almorzado</t>
+  </si>
+  <si>
+    <t>Recordá si vas a donar, tene en cuenta:</t>
+  </si>
+  <si>
+    <t>No te olvides de traer tu DNI Y tu lapicera</t>
   </si>
 </sst>
 </file>
@@ -599,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -692,6 +747,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -707,27 +768,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -737,52 +792,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,12 +852,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -806,6 +861,14 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1238,211 +1301,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1E719E-A3DA-467D-A9DC-CC79BFBD2FD0}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:I21"/>
+      <selection activeCell="K6" sqref="K6:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="0.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="49" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="I1" s="52"/>
+    </row>
+    <row r="2" spans="1:12" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="G3" s="48" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="G3" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="48"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-    </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
+      <c r="H3" s="50"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="K4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="K6" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="K7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="48"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+    </row>
+    <row r="12" spans="1:12" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="46"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="46"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="46"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
     </row>
     <row r="19" spans="1:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1460,6 +1542,187 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A7167A-80CE-441E-91EC-7AD184B2E397}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="48"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
+      <c r="E6" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="E8" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="E9" s="71" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="41"/>
+      <c r="F12" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="42"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="45"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A15:I16"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B9"/>
+    <mergeCell ref="E6:I7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="F12:H12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9150777F-3A1E-42AF-9C97-AE5D9A75BFA3}">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -1652,28 +1915,28 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1686,7 +1949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B6DFDB-A149-40D5-B71D-E57FE0C4F465}">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -1879,28 +2142,28 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1913,7 +2176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DE2BAE-38F0-4D1E-9387-7962FAC31A67}">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -1954,53 +2217,53 @@
       <c r="C3" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62" t="s">
+      <c r="F5" s="71"/>
+      <c r="G5" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6" s="62" t="s">
+      <c r="E6" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62" t="s">
+      <c r="F6" s="71"/>
+      <c r="G6" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62" t="s">
+      <c r="F7" s="71"/>
+      <c r="G7" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" s="38"/>
@@ -2011,11 +2274,11 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9" s="41"/>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
       <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2026,31 +2289,32 @@
       <c r="I10" s="45"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:I13"/>
     <mergeCell ref="E3:I4"/>
     <mergeCell ref="E5:F5"/>
@@ -2060,7 +2324,6 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="F9:H9"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2071,7 +2334,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,10 +2344,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="4"/>
       <c r="D1" s="3" t="s">
         <v>15</v>
@@ -2111,12 +2374,12 @@
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -2124,91 +2387,91 @@
       <c r="I3" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="54"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="54"/>
-      <c r="G5" s="54" t="s">
+      <c r="E5" s="55"/>
+      <c r="G5" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="54"/>
+      <c r="H5" s="55"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="G6" s="55" t="s">
+      <c r="E6" s="56"/>
+      <c r="G6" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="55"/>
+      <c r="H6" s="56"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
-      <c r="B9" s="55"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="53"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="53"/>
-      <c r="G10" s="53" t="s">
+      <c r="E10" s="57"/>
+      <c r="G10" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="53"/>
+      <c r="H10" s="57"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="46"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="G11" s="46" t="s">
+      <c r="E11" s="48"/>
+      <c r="G11" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="46"/>
+      <c r="H11" s="48"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
@@ -2229,134 +2492,135 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="D14" s="54" t="s">
+      <c r="B14" s="55"/>
+      <c r="D14" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="54"/>
-      <c r="G14" s="54" t="s">
+      <c r="E14" s="55"/>
+      <c r="G14" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="54"/>
+      <c r="H14" s="55"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="55"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="55"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="55" t="s">
+      <c r="G15" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="55"/>
+      <c r="H15" s="56"/>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="53"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="53" t="s">
+      <c r="D19" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="53"/>
+      <c r="E19" s="57"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="53" t="s">
+      <c r="G19" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="53"/>
+      <c r="H19" s="57"/>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="46"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="46"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="46"/>
+      <c r="H20" s="48"/>
       <c r="I20" s="6"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E9"/>
-    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G15:H18"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A15:B18"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="A22:I23"/>
     <mergeCell ref="A5:B5"/>
@@ -2373,12 +2637,11 @@
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A15:B18"/>
-    <mergeCell ref="G15:H18"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E9"/>
+    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2395,10 +2658,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="4"/>
       <c r="D1" s="3" t="s">
         <v>15</v>
@@ -2414,12 +2677,12 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
       <c r="H3" s="58"/>
@@ -2432,42 +2695,42 @@
       <c r="I4" s="58"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="F5" s="58"/>
       <c r="G5" s="58"/>
       <c r="H5" s="58"/>
       <c r="I5" s="58"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
       <c r="F6" s="58"/>
       <c r="G6" s="58"/>
       <c r="H6" s="58"/>
       <c r="I6" s="58"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="F7" s="58"/>
       <c r="G7" s="58"/>
       <c r="H7" s="58"/>
       <c r="I7" s="58"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
       <c r="F8" s="58"/>
       <c r="G8" s="58"/>
       <c r="H8" s="58"/>
@@ -2480,84 +2743,84 @@
       <c r="I9" s="58"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
       <c r="F10" s="58"/>
       <c r="G10" s="58"/>
       <c r="H10" s="58"/>
       <c r="I10" s="58"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
       <c r="F11" s="58"/>
       <c r="G11" s="58"/>
       <c r="H11" s="58"/>
       <c r="I11" s="58"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
       <c r="F12" s="58"/>
       <c r="G12" s="58"/>
       <c r="H12" s="58"/>
       <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
       <c r="F13" s="58"/>
       <c r="G13" s="58"/>
       <c r="H13" s="58"/>
       <c r="I13" s="58"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
       <c r="F14" s="58"/>
       <c r="G14" s="58"/>
       <c r="H14" s="58"/>
       <c r="I14" s="58"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
       <c r="F15" s="58"/>
       <c r="G15" s="58"/>
       <c r="H15" s="58"/>
       <c r="I15" s="58"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
       <c r="F18" s="59" t="s">
         <v>22</v>
       </c>
@@ -2565,37 +2828,37 @@
       <c r="H18" s="59"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
       <c r="F19" s="59"/>
       <c r="G19" s="59"/>
       <c r="H19" s="59"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2614,10 +2877,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C922557-EDD8-4102-B48D-EC2817759495}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2625,11 +2888,11 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="4"/>
       <c r="D1" s="3" t="s">
         <v>15</v>
@@ -2644,7 +2907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>21</v>
       </c>
@@ -2666,8 +2929,11 @@
       <c r="I3" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>21</v>
       </c>
@@ -2689,8 +2955,11 @@
       <c r="I4" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>21</v>
       </c>
@@ -2713,7 +2982,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>21</v>
       </c>
@@ -2736,7 +3005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
         <v>21</v>
       </c>
@@ -2759,7 +3028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
         <v>21</v>
       </c>
@@ -2782,7 +3051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>21</v>
       </c>
@@ -2805,32 +3074,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:I13"/>
     <mergeCell ref="C3:D3"/>
@@ -2847,23 +3123,208 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F03EA77-8C8D-4243-828A-BC9DFC99851B}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="84"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="86"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="84" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="84"/>
+      <c r="C6" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="86"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="84" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="84" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="86"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="84" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="84"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:I13"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3AEC875-5414-4CC3-A789-DB7AB4C1088C}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2874,10 +3335,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="3" t="s">
@@ -2893,18 +3354,18 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="E3" s="46" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="E3" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -2916,67 +3377,67 @@
       <c r="C4" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="64"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="66"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="66"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="66"/>
+      <c r="C9" s="68"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -2991,53 +3452,53 @@
       <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="E11" s="67" t="s">
+      <c r="B11" s="48"/>
+      <c r="E11" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
-      <c r="E13" s="62" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="E13" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62" t="s">
+      <c r="F13" s="71"/>
+      <c r="G13" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62" t="s">
+      <c r="F14" s="71"/>
+      <c r="G14" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -3054,15 +3515,15 @@
       <c r="C15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="62" t="s">
+      <c r="E15" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62" t="s">
+      <c r="F15" s="71"/>
+      <c r="G15" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
@@ -3101,11 +3562,11 @@
         <v>33</v>
       </c>
       <c r="E17" s="41"/>
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
       <c r="I17" s="42"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3125,31 +3586,32 @@
       <c r="I18" s="45"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G15:I15"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A20:I21"/>
     <mergeCell ref="A11:B13"/>
@@ -3166,18 +3628,17 @@
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1C89C7-6D77-45FB-99A0-F6C0D6A704A8}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3191,10 +3652,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="74"/>
       <c r="C1" s="15"/>
       <c r="D1" s="14" t="s">
         <v>16</v>
@@ -3218,19 +3679,19 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
       <c r="K4" s="3" t="s">
         <v>41</v>
       </c>
@@ -3238,29 +3699,29 @@
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="61" t="s">
+      <c r="F5" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="74" t="s">
+      <c r="G5" s="70"/>
+      <c r="H5" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="75"/>
+      <c r="I5" s="73"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="61"/>
-      <c r="H6" s="74" t="s">
+      <c r="G6" s="70"/>
+      <c r="H6" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="75"/>
+      <c r="I6" s="73"/>
       <c r="K6" s="2" t="s">
         <v>42</v>
       </c>
@@ -3275,14 +3736,14 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F7" s="61" t="s">
+      <c r="F7" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="61"/>
-      <c r="H7" s="74" t="s">
+      <c r="G7" s="70"/>
+      <c r="H7" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="75"/>
+      <c r="I7" s="73"/>
       <c r="K7" s="12" t="s">
         <v>46</v>
       </c>
@@ -3312,24 +3773,24 @@
       <c r="C8" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="61" t="s">
+      <c r="F8" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="74" t="s">
+      <c r="G8" s="70"/>
+      <c r="H8" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="75"/>
+      <c r="I8" s="73"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="61"/>
-      <c r="H9" s="74" t="s">
+      <c r="G9" s="70"/>
+      <c r="H9" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="75"/>
+      <c r="I9" s="73"/>
       <c r="K9" s="2" t="s">
         <v>42</v>
       </c>
@@ -3353,14 +3814,14 @@
       <c r="C10" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="61" t="s">
+      <c r="F10" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="61"/>
-      <c r="H10" s="74" t="s">
+      <c r="G10" s="70"/>
+      <c r="H10" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="75"/>
+      <c r="I10" s="73"/>
       <c r="K10" s="12" t="s">
         <v>46</v>
       </c>
@@ -3379,14 +3840,14 @@
       <c r="Q10" s="60"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F11" s="61" t="s">
+      <c r="F11" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="61"/>
-      <c r="H11" s="74" t="s">
+      <c r="G11" s="70"/>
+      <c r="H11" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="75"/>
+      <c r="I11" s="73"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
@@ -3398,34 +3859,34 @@
       <c r="C12" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="61" t="s">
+      <c r="F12" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="61"/>
-      <c r="H12" s="74" t="s">
+      <c r="G12" s="70"/>
+      <c r="H12" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="75"/>
+      <c r="I12" s="73"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F13" s="61" t="s">
+      <c r="F13" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="61"/>
-      <c r="H13" s="74" t="s">
+      <c r="G13" s="70"/>
+      <c r="H13" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="75"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F14" s="61" t="s">
+      <c r="F14" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="61"/>
-      <c r="H14" s="74" t="s">
+      <c r="G14" s="70"/>
+      <c r="H14" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="75"/>
+      <c r="I14" s="73"/>
       <c r="K14" t="s">
         <v>51</v>
       </c>
@@ -3445,17 +3906,17 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
       <c r="K16">
         <v>1</v>
       </c>
@@ -3470,18 +3931,30 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="H14:I14"/>
@@ -3491,42 +3964,30 @@
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="A4:C5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157DE640-FC3A-4E15-A23C-B0FDCE3ADBF6}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="74"/>
       <c r="C1" s="15"/>
       <c r="D1" s="14" t="s">
         <v>16</v>
@@ -3718,28 +4179,28 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3750,7 +4211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9105B367-AF6B-481E-A20D-27E1DDD6A1ED}">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -3761,10 +4222,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="78"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29" t="s">
         <v>16</v>
@@ -3782,20 +4243,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="73"/>
+      <c r="B3" s="75"/>
       <c r="C3" s="60" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="60"/>
       <c r="E3" s="60"/>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G4" s="12"/>
@@ -3803,10 +4264,10 @@
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="73"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="60" t="s">
         <v>71</v>
       </c>
@@ -3815,10 +4276,10 @@
       <c r="G5" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="77" t="s">
+      <c r="H5" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="78"/>
+      <c r="I5" s="80"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G6" s="12"/>
@@ -3826,10 +4287,10 @@
       <c r="I6" s="32"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="73"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="60" t="s">
         <v>71</v>
       </c>
@@ -3838,10 +4299,10 @@
       <c r="G7" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="77" t="s">
+      <c r="H7" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="I7" s="78"/>
+      <c r="I7" s="80"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" s="12"/>
@@ -3849,10 +4310,10 @@
       <c r="I8" s="32"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="73"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="60" t="s">
         <v>71</v>
       </c>
@@ -3861,10 +4322,10 @@
       <c r="G9" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="I9" s="78"/>
+      <c r="I9" s="80"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G10" s="12"/>
@@ -3872,10 +4333,10 @@
       <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="73"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="60" t="s">
         <v>71</v>
       </c>
@@ -3884,51 +4345,57 @@
       <c r="G11" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="78"/>
+      <c r="I11" s="80"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="70"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="63"/>
       <c r="G13" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="77" t="s">
+      <c r="H13" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="78"/>
+      <c r="I13" s="80"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="A15:I16"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -3942,193 +4409,6 @@
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H9:I9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A7167A-80CE-441E-91EC-7AD184B2E397}">
-  <dimension ref="A1:I16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:I13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="46"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="E6" s="67" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="E8" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="E9" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="62" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="41"/>
-      <c r="F12" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="42"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="45"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-    </row>
-  </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A15:I16"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B9"/>
-    <mergeCell ref="E6:I7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>